<commit_message>
feat: new dk ver 1.0
</commit_message>
<xml_diff>
--- a/ReinforcementLearning/output.xlsx
+++ b/ReinforcementLearning/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CT98"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,566 +432,566 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
-      </c>
-      <c r="C3" t="n">
-        <v>85</v>
-      </c>
-      <c r="D3" t="n">
-        <v>57</v>
-      </c>
-      <c r="E3" t="n">
-        <v>81</v>
-      </c>
-      <c r="F3" t="n">
-        <v>40</v>
-      </c>
-      <c r="G3" t="n">
-        <v>64</v>
-      </c>
-      <c r="H3" t="n">
-        <v>66</v>
-      </c>
-      <c r="I3" t="n">
-        <v>71</v>
-      </c>
-      <c r="J3" t="n">
-        <v>77</v>
-      </c>
-      <c r="K3" t="n">
-        <v>79</v>
-      </c>
-      <c r="L3" t="n">
-        <v>67</v>
-      </c>
-      <c r="M3" t="n">
-        <v>93</v>
-      </c>
-      <c r="N3" t="n">
-        <v>70</v>
-      </c>
-      <c r="O3" t="n">
-        <v>26</v>
-      </c>
-      <c r="P3" t="n">
-        <v>7</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>16</v>
-      </c>
-      <c r="R3" t="n">
-        <v>84</v>
-      </c>
-      <c r="S3" t="n">
-        <v>83</v>
-      </c>
-      <c r="T3" t="n">
-        <v>8</v>
-      </c>
-      <c r="U3" t="n">
-        <v>49</v>
-      </c>
-      <c r="V3" t="n">
-        <v>86</v>
-      </c>
-      <c r="W3" t="n">
-        <v>47</v>
-      </c>
-      <c r="X3" t="n">
-        <v>30</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>4</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>58</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>37</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>13</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>46</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>35</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>96</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>61</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>78</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>75</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>44</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>22</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>36</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>50</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>69</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>15</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>89</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>56</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>90</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>18</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>87</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>6</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>29</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>34</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>28</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>32</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>43</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>62</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>42</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>14</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>91</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>94</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>52</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>5</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>21</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>39</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>65</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>10</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>53</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>19</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>80</v>
-      </c>
-      <c r="BP3" t="n">
-        <v>45</v>
-      </c>
-      <c r="BQ3" t="n">
-        <v>59</v>
-      </c>
-      <c r="BR3" t="n">
-        <v>31</v>
-      </c>
-      <c r="BS3" t="n">
-        <v>74</v>
-      </c>
-      <c r="BT3" t="n">
-        <v>72</v>
-      </c>
-      <c r="BU3" t="n">
-        <v>68</v>
-      </c>
-      <c r="BV3" t="n">
-        <v>20</v>
-      </c>
-      <c r="BW3" t="n">
         <v>63</v>
-      </c>
-      <c r="BX3" t="n">
-        <v>60</v>
-      </c>
-      <c r="BY3" t="n">
-        <v>17</v>
-      </c>
-      <c r="BZ3" t="n">
-        <v>48</v>
-      </c>
-      <c r="CA3" t="n">
-        <v>76</v>
-      </c>
-      <c r="CB3" t="n">
-        <v>33</v>
-      </c>
-      <c r="CC3" t="n">
-        <v>23</v>
-      </c>
-      <c r="CD3" t="n">
-        <v>95</v>
-      </c>
-      <c r="CE3" t="n">
-        <v>3</v>
-      </c>
-      <c r="CF3" t="n">
-        <v>88</v>
-      </c>
-      <c r="CG3" t="n">
-        <v>27</v>
-      </c>
-      <c r="CH3" t="n">
-        <v>25</v>
-      </c>
-      <c r="CI3" t="n">
-        <v>38</v>
-      </c>
-      <c r="CJ3" t="n">
-        <v>51</v>
-      </c>
-      <c r="CK3" t="n">
-        <v>24</v>
-      </c>
-      <c r="CL3" t="n">
-        <v>1</v>
-      </c>
-      <c r="CM3" t="n">
-        <v>9</v>
-      </c>
-      <c r="CN3" t="n">
-        <v>92</v>
-      </c>
-      <c r="CO3" t="n">
-        <v>11</v>
-      </c>
-      <c r="CP3" t="n">
-        <v>55</v>
-      </c>
-      <c r="CQ3" t="n">
-        <v>82</v>
-      </c>
-      <c r="CR3" t="n">
-        <v>54</v>
-      </c>
-      <c r="CS3" t="n">
-        <v>41</v>
-      </c>
-      <c r="CT3" t="n">
-        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
+      <c r="B4" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
+      <c r="B5" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" t="n">
+        <v>86</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
+      <c r="B6" t="n">
+        <v>70</v>
+      </c>
+      <c r="C6" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
+      <c r="B7" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
+      <c r="B8" t="n">
+        <v>90</v>
+      </c>
+      <c r="C8" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
       </c>
+      <c r="B9" t="n">
+        <v>85</v>
+      </c>
+      <c r="C9" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
         <v>9</v>
       </c>
+      <c r="B10" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
+      <c r="B11" t="n">
+        <v>45</v>
+      </c>
+      <c r="C11" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
+      <c r="B12" t="n">
+        <v>71</v>
+      </c>
+      <c r="C12" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
+      <c r="B13" t="n">
+        <v>74</v>
+      </c>
+      <c r="C13" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="n">
+        <v>24</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>80</v>
+      </c>
+      <c r="C16" t="n">
+        <v>52</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
+      <c r="B18" t="n">
+        <v>39</v>
+      </c>
+      <c r="C18" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>47</v>
+      </c>
+      <c r="C21" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
+      <c r="B22" t="n">
+        <v>61</v>
+      </c>
+      <c r="C22" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
+      <c r="B23" t="n">
+        <v>65</v>
+      </c>
+      <c r="C23" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
+      <c r="B24" t="n">
+        <v>55</v>
+      </c>
+      <c r="C24" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>24</v>
       </c>
+      <c r="B25" t="n">
+        <v>7</v>
+      </c>
+      <c r="C25" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
         <v>25</v>
       </c>
+      <c r="B26" t="n">
+        <v>32</v>
+      </c>
+      <c r="C26" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
         <v>26</v>
       </c>
+      <c r="B27" t="n">
+        <v>81</v>
+      </c>
+      <c r="C27" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
         <v>27</v>
       </c>
+      <c r="B28" t="n">
+        <v>58</v>
+      </c>
+      <c r="C28" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
         <v>28</v>
       </c>
+      <c r="B29" t="n">
+        <v>87</v>
+      </c>
+      <c r="C29" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
         <v>29</v>
       </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
         <v>30</v>
       </c>
+      <c r="B31" t="n">
+        <v>67</v>
+      </c>
+      <c r="C31" t="n">
+        <v>66</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
         <v>31</v>
       </c>
+      <c r="B32" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
         <v>32</v>
       </c>
+      <c r="B33" t="n">
+        <v>9</v>
+      </c>
+      <c r="C33" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
         <v>33</v>
       </c>
+      <c r="B34" t="n">
+        <v>83</v>
+      </c>
+      <c r="C34" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>34</v>
       </c>
+      <c r="B35" t="n">
+        <v>15</v>
+      </c>
+      <c r="C35" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
         <v>35</v>
       </c>
+      <c r="B36" t="n">
+        <v>53</v>
+      </c>
+      <c r="C36" t="n">
+        <v>78</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
         <v>36</v>
       </c>
+      <c r="B37" t="n">
+        <v>22</v>
+      </c>
+      <c r="C37" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
         <v>37</v>
       </c>
+      <c r="B38" t="n">
+        <v>36</v>
+      </c>
+      <c r="C38" t="n">
+        <v>93</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>38</v>
       </c>
+      <c r="B39" t="n">
+        <v>88</v>
+      </c>
+      <c r="C39" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
         <v>39</v>
       </c>
+      <c r="B40" t="n">
+        <v>72</v>
+      </c>
+      <c r="C40" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
         <v>40</v>
       </c>
+      <c r="B41" t="n">
+        <v>25</v>
+      </c>
+      <c r="C41" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
         <v>41</v>
       </c>
+      <c r="B42" t="n">
+        <v>75</v>
+      </c>
+      <c r="C42" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>42</v>
       </c>
+      <c r="B43" t="n">
+        <v>40</v>
+      </c>
+      <c r="C43" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
         <v>43</v>
       </c>
+      <c r="B44" t="n">
+        <v>91</v>
+      </c>
+      <c r="C44" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
         <v>44</v>
       </c>
+      <c r="B45" t="n">
+        <v>48</v>
+      </c>
+      <c r="C45" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>45</v>
       </c>
+      <c r="B46" t="n">
+        <v>94</v>
+      </c>
+      <c r="C46" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
         <v>46</v>
       </c>
+      <c r="B47" t="n">
+        <v>79</v>
+      </c>
+      <c r="C47" t="n">
+        <v>76</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
         <v>47</v>
       </c>
+      <c r="B48" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>48</v>
       </c>
+      <c r="B49" t="n">
+        <v>57</v>
+      </c>
+      <c r="C49" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>49</v>
       </c>
+      <c r="B50" t="n">
+        <v>89</v>
+      </c>
+      <c r="C50" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>50</v>
       </c>
+      <c r="B51" t="n">
+        <v>69</v>
+      </c>
+      <c r="C51" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
         <v>51</v>
       </c>
+      <c r="B52" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
         <v>52</v>
       </c>
+      <c r="B53" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
         <v>53</v>
       </c>
+      <c r="B54" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
         <v>54</v>
       </c>
+      <c r="B55" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>55</v>
+      </c>
+      <c r="B56" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="57">

</xml_diff>